<commit_message>
last cp data up
</commit_message>
<xml_diff>
--- a/demos/cp/cp.xlsx
+++ b/demos/cp/cp.xlsx
@@ -866,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO105"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U72" sqref="U72"/>
+    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -5586,7 +5586,7 @@
         <v>3</v>
       </c>
       <c r="P47" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q47" s="7">
         <v>7</v>
@@ -6065,7 +6065,7 @@
         <v>7</v>
       </c>
       <c r="J52" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="7">
         <v>0</v>
@@ -6358,7 +6358,9 @@
         <v>13</v>
       </c>
       <c r="J55" s="7"/>
-      <c r="K55" s="7"/>
+      <c r="K55" s="7">
+        <v>0</v>
+      </c>
       <c r="L55" s="7">
         <v>1</v>
       </c>
@@ -6378,7 +6380,7 @@
       <c r="R55" s="7">
         <v>5</v>
       </c>
-      <c r="S55" s="25">
+      <c r="S55" s="7">
         <v>2</v>
       </c>
       <c r="T55" s="7">
@@ -6391,7 +6393,7 @@
         <v>3</v>
       </c>
       <c r="W55" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X55" s="7">
         <v>17</v>
@@ -6412,7 +6414,7 @@
         <v>7</v>
       </c>
       <c r="AD55" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AE55" s="7">
         <v>11</v>
@@ -6425,7 +6427,9 @@
       </c>
     </row>
     <row r="56" spans="1:33" s="25" customFormat="1">
-      <c r="A56" s="7"/>
+      <c r="A56" s="7">
+        <v>0</v>
+      </c>
       <c r="B56" s="7">
         <v>0</v>
       </c>
@@ -6471,7 +6475,7 @@
       <c r="R56" s="7">
         <v>1</v>
       </c>
-      <c r="S56" s="25">
+      <c r="S56" s="7">
         <v>6</v>
       </c>
       <c r="T56" s="7">
@@ -6557,9 +6561,9 @@
         <v>0</v>
       </c>
       <c r="R57" s="7">
-        <v>4</v>
-      </c>
-      <c r="S57" s="25">
+        <v>5</v>
+      </c>
+      <c r="S57" s="7">
         <v>2</v>
       </c>
       <c r="T57" s="7">
@@ -6592,7 +6596,7 @@
       </c>
       <c r="AD57" s="7"/>
       <c r="AE57" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF57" s="7">
         <v>2</v>
@@ -6607,7 +6611,7 @@
         <v>6</v>
       </c>
       <c r="C58" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D58" s="7">
         <v>0</v>
@@ -6646,13 +6650,15 @@
         <v>0</v>
       </c>
       <c r="R58" s="7"/>
-      <c r="S58" s="25">
+      <c r="S58" s="7">
         <v>3</v>
       </c>
       <c r="T58" s="7">
         <v>0</v>
       </c>
-      <c r="U58" s="7"/>
+      <c r="U58" s="7">
+        <v>0</v>
+      </c>
       <c r="V58" s="7">
         <v>7</v>
       </c>
@@ -6681,7 +6687,7 @@
         <v>6</v>
       </c>
       <c r="AG58" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:33" s="7" customFormat="1">
@@ -6727,7 +6733,7 @@
         <v>2</v>
       </c>
       <c r="T59" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V59" s="7">
         <v>4</v>
@@ -6772,8 +6778,11 @@
       <c r="G60" s="7">
         <v>9</v>
       </c>
+      <c r="H60" s="7">
+        <v>0</v>
+      </c>
       <c r="I60" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L60" s="7">
         <v>3</v>
@@ -6782,7 +6791,7 @@
         <v>2</v>
       </c>
       <c r="N60" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O60" s="7">
         <v>8</v>
@@ -6800,7 +6809,7 @@
         <v>0</v>
       </c>
       <c r="Y60" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z60" s="7">
         <v>2</v>
@@ -6812,7 +6821,7 @@
         <v>16</v>
       </c>
       <c r="AC60" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF60" s="7">
         <v>3</v>
@@ -6873,7 +6882,7 @@
         <v>8</v>
       </c>
       <c r="AA61" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB61" s="7">
         <v>12</v>
@@ -6888,7 +6897,7 @@
     <row r="62" spans="1:33">
       <c r="A62" s="7"/>
       <c r="B62" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7">
@@ -6908,7 +6917,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M62" s="7">
         <v>4</v>
@@ -6946,7 +6955,7 @@
       <c r="AD62" s="7"/>
       <c r="AE62" s="3"/>
       <c r="AF62" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG62" s="27"/>
     </row>
@@ -6960,10 +6969,10 @@
         <v>7</v>
       </c>
       <c r="F63" s="41">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G63" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H63" s="4"/>
       <c r="J63" s="3"/>
@@ -6981,7 +6990,9 @@
         <v>2</v>
       </c>
       <c r="R63" s="7"/>
-      <c r="S63" s="4"/>
+      <c r="S63" s="4">
+        <v>0</v>
+      </c>
       <c r="T63" s="3"/>
       <c r="U63" s="4"/>
       <c r="V63" s="4">
@@ -7021,7 +7032,7 @@
       </c>
       <c r="N64" s="4"/>
       <c r="O64" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P64" s="4"/>
       <c r="Q64" s="4">
@@ -7080,10 +7091,12 @@
         <v>9</v>
       </c>
       <c r="W65" s="4"/>
-      <c r="X65" s="4"/>
+      <c r="X65" s="4">
+        <v>0</v>
+      </c>
       <c r="Y65" s="4"/>
       <c r="Z65" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AB65" s="7">
         <v>3</v>
@@ -7118,14 +7131,14 @@
       <c r="T66" s="3"/>
       <c r="U66" s="4"/>
       <c r="V66" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="W66" s="4"/>
       <c r="X66" s="4"/>
       <c r="Y66" s="4"/>
       <c r="Z66" s="4"/>
       <c r="AB66" s="14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AD66" s="4"/>
       <c r="AE66" s="3"/>
@@ -7185,7 +7198,7 @@
       <c r="N68" s="4"/>
       <c r="O68" s="4"/>
       <c r="Q68" s="41">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R68" s="4"/>
       <c r="S68" s="4"/>
@@ -7206,7 +7219,7 @@
         <v>3</v>
       </c>
       <c r="E69" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F69" s="4"/>
       <c r="H69" s="4"/>
@@ -7214,7 +7227,7 @@
       <c r="J69" s="3"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
@@ -7295,7 +7308,7 @@
     </row>
     <row r="72" spans="1:33">
       <c r="D72" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
@@ -7888,8 +7901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT970"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B145" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E175" sqref="E175"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J173" sqref="J173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
@@ -19633,7 +19646,7 @@
       </c>
       <c r="P147" s="22"/>
       <c r="Q147" s="20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R147" s="19">
         <v>2</v>
@@ -19952,7 +19965,7 @@
         <v>7</v>
       </c>
       <c r="U150" s="20">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V150" s="19">
         <v>1</v>
@@ -20652,12 +20665,12 @@
       </c>
       <c r="P157" s="22"/>
       <c r="Q157" s="20">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R157" s="19">
         <v>3</v>
       </c>
-      <c r="S157" s="20">
+      <c r="S157" s="19">
         <v>8</v>
       </c>
       <c r="T157" s="19">
@@ -20682,7 +20695,9 @@
       <c r="AA157" s="19">
         <v>4</v>
       </c>
-      <c r="AB157" s="20"/>
+      <c r="AB157" s="19">
+        <v>8</v>
+      </c>
       <c r="AC157" s="20"/>
       <c r="AD157" s="20"/>
       <c r="AF157" s="40"/>
@@ -20752,7 +20767,7 @@
         <v>9</v>
       </c>
       <c r="P158" s="22"/>
-      <c r="Q158" s="23">
+      <c r="Q158" s="22">
         <v>7</v>
       </c>
       <c r="R158" s="22">
@@ -20762,9 +20777,9 @@
         <v>4</v>
       </c>
       <c r="T158" s="23">
-        <v>7</v>
-      </c>
-      <c r="U158" s="23">
+        <v>8</v>
+      </c>
+      <c r="U158" s="22">
         <v>7</v>
       </c>
       <c r="V158" s="22">
@@ -20780,8 +20795,12 @@
       <c r="Z158" s="19">
         <v>4</v>
       </c>
-      <c r="AA158" s="23"/>
-      <c r="AB158" s="23"/>
+      <c r="AA158" s="19">
+        <v>7</v>
+      </c>
+      <c r="AB158" s="19">
+        <v>7</v>
+      </c>
       <c r="AC158" s="23"/>
       <c r="AD158" s="23"/>
       <c r="AF158" s="40"/>
@@ -20846,13 +20865,13 @@
       </c>
       <c r="P159" s="22"/>
       <c r="Q159" s="20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R159" s="19">
         <v>1</v>
       </c>
       <c r="S159" s="20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="T159" s="19">
         <v>0</v>
@@ -20941,22 +20960,22 @@
       </c>
       <c r="P160" s="22"/>
       <c r="Q160" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R160" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S160" s="19">
         <v>3</v>
       </c>
       <c r="T160" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U160" s="19">
         <v>1</v>
       </c>
       <c r="V160" s="20">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W160" s="20"/>
       <c r="X160" s="19">
@@ -21044,16 +21063,16 @@
         <v>3</v>
       </c>
       <c r="S161" s="20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T161" s="19">
         <v>0</v>
       </c>
       <c r="U161" s="20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V161" s="20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W161" s="15"/>
       <c r="X161" s="19">
@@ -21140,16 +21159,16 @@
         <v>2</v>
       </c>
       <c r="S162" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T162" s="19">
         <v>2</v>
       </c>
       <c r="U162" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V162" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W162" s="20"/>
       <c r="X162" s="22">
@@ -21238,20 +21257,20 @@
       <c r="R163" s="22">
         <v>1</v>
       </c>
-      <c r="S163" s="23">
+      <c r="S163" s="22">
         <v>2</v>
       </c>
       <c r="T163" s="22">
         <v>0</v>
       </c>
       <c r="U163" s="23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V163" s="22">
         <v>1</v>
       </c>
       <c r="W163" s="23"/>
-      <c r="X163" s="21">
+      <c r="X163" s="22">
         <v>0</v>
       </c>
       <c r="Y163" s="22">
@@ -21263,7 +21282,9 @@
       <c r="AA163" s="19">
         <v>1</v>
       </c>
-      <c r="AB163" s="23"/>
+      <c r="AB163" s="19">
+        <v>2</v>
+      </c>
       <c r="AC163" s="23"/>
       <c r="AD163" s="23"/>
       <c r="AF163" s="40"/>
@@ -21328,31 +21349,33 @@
       </c>
       <c r="P164" s="22"/>
       <c r="Q164" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R164" s="20">
-        <v>1</v>
-      </c>
-      <c r="S164" s="20">
+        <v>2</v>
+      </c>
+      <c r="S164" s="22">
         <v>1</v>
       </c>
       <c r="T164" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U164" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V164" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W164" s="20"/>
-      <c r="X164" s="20"/>
+      <c r="X164" s="19">
+        <v>1</v>
+      </c>
       <c r="Y164" s="20"/>
       <c r="Z164" s="20"/>
       <c r="AA164" s="20"/>
       <c r="AB164" s="20"/>
       <c r="AC164" s="20"/>
-      <c r="AD164" s="15"/>
+      <c r="AD164" s="20"/>
       <c r="AF164" s="40"/>
       <c r="AH164" s="21">
         <v>0</v>
@@ -21418,25 +21441,27 @@
       </c>
       <c r="P165" s="22"/>
       <c r="Q165" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R165" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S165" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T165" s="20">
-        <v>0</v>
-      </c>
-      <c r="U165" s="20">
+        <v>1</v>
+      </c>
+      <c r="U165" s="19">
         <v>0</v>
       </c>
       <c r="V165" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W165" s="20"/>
-      <c r="X165" s="20"/>
+      <c r="X165" s="19">
+        <v>0</v>
+      </c>
       <c r="Y165" s="20"/>
       <c r="Z165" s="20"/>
       <c r="AA165" s="20"/>
@@ -21467,22 +21492,94 @@
       </c>
     </row>
     <row r="166" spans="1:43" s="21" customFormat="1">
+      <c r="A166" s="21">
+        <v>7</v>
+      </c>
+      <c r="B166" s="21">
+        <v>1</v>
+      </c>
+      <c r="C166" s="21">
+        <v>8</v>
+      </c>
+      <c r="D166" s="21">
+        <v>2</v>
+      </c>
+      <c r="E166" s="21">
+        <v>0</v>
+      </c>
+      <c r="F166" s="21">
+        <v>7</v>
+      </c>
+      <c r="I166" s="21">
+        <v>0</v>
+      </c>
+      <c r="J166" s="21">
+        <v>1</v>
+      </c>
+      <c r="K166" s="21">
+        <v>2</v>
+      </c>
+      <c r="L166" s="21">
+        <v>7</v>
+      </c>
+      <c r="M166" s="21">
+        <v>7</v>
+      </c>
+      <c r="N166" s="21">
+        <v>8</v>
+      </c>
       <c r="P166" s="22"/>
-      <c r="Q166" s="20"/>
-      <c r="R166" s="20"/>
-      <c r="S166" s="20"/>
-      <c r="T166" s="20"/>
-      <c r="U166" s="20"/>
-      <c r="V166" s="20"/>
-      <c r="W166" s="15"/>
-      <c r="X166" s="15"/>
+      <c r="Q166" s="20">
+        <v>0</v>
+      </c>
+      <c r="R166" s="20">
+        <v>0</v>
+      </c>
+      <c r="S166" s="20">
+        <v>0</v>
+      </c>
+      <c r="T166" s="20">
+        <v>0</v>
+      </c>
+      <c r="U166" s="20">
+        <v>0</v>
+      </c>
+      <c r="V166" s="20">
+        <v>0</v>
+      </c>
+      <c r="W166" s="20"/>
+      <c r="X166" s="20"/>
       <c r="Y166" s="20"/>
       <c r="Z166" s="20"/>
       <c r="AA166" s="20"/>
       <c r="AB166" s="20"/>
       <c r="AC166" s="20"/>
-      <c r="AD166" s="15"/>
+      <c r="AD166" s="20"/>
       <c r="AF166" s="40"/>
+      <c r="AH166" s="21">
+        <v>0</v>
+      </c>
+      <c r="AI166" s="21">
+        <v>1</v>
+      </c>
+      <c r="AJ166" s="21">
+        <v>2</v>
+      </c>
+      <c r="AK166" s="21">
+        <v>7</v>
+      </c>
+      <c r="AL166" s="21">
+        <v>8</v>
+      </c>
+      <c r="AO166" s="21">
+        <v>2</v>
+      </c>
+      <c r="AP166" s="21">
+        <v>1</v>
+      </c>
+      <c r="AQ166" s="21">
+        <v>2</v>
+      </c>
     </row>
     <row r="167" spans="1:43" s="21" customFormat="1">
       <c r="P167" s="22"/>
@@ -21521,7 +21618,6 @@
       <c r="AF168" s="40"/>
     </row>
     <row r="169" spans="1:43" s="21" customFormat="1">
-      <c r="P169" s="22"/>
       <c r="Q169" s="20"/>
       <c r="R169" s="20"/>
       <c r="S169" s="20"/>
@@ -21529,34 +21625,34 @@
       <c r="U169" s="20"/>
       <c r="V169" s="20"/>
       <c r="W169" s="20"/>
-      <c r="X169" s="15"/>
+      <c r="X169" s="20"/>
       <c r="Y169" s="20"/>
       <c r="Z169" s="20"/>
       <c r="AA169" s="20"/>
       <c r="AB169" s="20"/>
       <c r="AC169" s="20"/>
-      <c r="AD169" s="15"/>
+      <c r="AD169" s="20"/>
       <c r="AF169" s="40"/>
     </row>
     <row r="170" spans="1:43" s="21" customFormat="1">
-      <c r="Q170" s="20"/>
-      <c r="R170" s="20"/>
-      <c r="S170" s="20"/>
-      <c r="T170" s="20"/>
-      <c r="U170" s="20"/>
-      <c r="V170" s="20"/>
-      <c r="W170" s="20"/>
-      <c r="X170" s="20"/>
-      <c r="Y170" s="20"/>
-      <c r="Z170" s="20"/>
-      <c r="AA170" s="20"/>
-      <c r="AB170" s="20"/>
-      <c r="AC170" s="20"/>
-      <c r="AD170" s="15"/>
+      <c r="P170" s="22"/>
+      <c r="Q170" s="23"/>
+      <c r="R170" s="23"/>
+      <c r="S170" s="23"/>
+      <c r="T170" s="23"/>
+      <c r="U170" s="23"/>
+      <c r="V170" s="23"/>
+      <c r="W170" s="40"/>
+      <c r="X170" s="23"/>
+      <c r="Y170" s="23"/>
+      <c r="Z170" s="23"/>
+      <c r="AA170" s="23"/>
+      <c r="AB170" s="23"/>
+      <c r="AC170" s="23"/>
+      <c r="AD170" s="23"/>
       <c r="AF170" s="40"/>
     </row>
     <row r="171" spans="1:43" s="21" customFormat="1">
-      <c r="P171" s="22"/>
       <c r="Q171" s="23"/>
       <c r="R171" s="23"/>
       <c r="S171" s="23"/>
@@ -21597,13 +21693,13 @@
       <c r="T173" s="23"/>
       <c r="U173" s="23"/>
       <c r="V173" s="23"/>
-      <c r="W173" s="40"/>
+      <c r="W173" s="23"/>
       <c r="X173" s="40"/>
       <c r="Y173" s="40"/>
-      <c r="Z173" s="40"/>
-      <c r="AA173" s="40"/>
-      <c r="AB173" s="40"/>
-      <c r="AC173" s="40"/>
+      <c r="Z173" s="23"/>
+      <c r="AA173" s="23"/>
+      <c r="AB173" s="23"/>
+      <c r="AC173" s="23"/>
       <c r="AD173" s="40"/>
       <c r="AF173" s="40"/>
     </row>
@@ -21617,14 +21713,15 @@
       <c r="W174" s="23"/>
       <c r="X174" s="40"/>
       <c r="Y174" s="40"/>
-      <c r="Z174" s="23"/>
-      <c r="AA174" s="23"/>
-      <c r="AB174" s="23"/>
-      <c r="AC174" s="23"/>
+      <c r="Z174" s="40"/>
+      <c r="AA174" s="40"/>
+      <c r="AB174" s="40"/>
+      <c r="AC174" s="40"/>
       <c r="AD174" s="40"/>
       <c r="AF174" s="40"/>
     </row>
     <row r="175" spans="1:43" s="21" customFormat="1">
+      <c r="P175" s="22"/>
       <c r="Q175" s="23"/>
       <c r="R175" s="23"/>
       <c r="S175" s="23"/>
@@ -21634,15 +21731,14 @@
       <c r="W175" s="23"/>
       <c r="X175" s="40"/>
       <c r="Y175" s="40"/>
-      <c r="Z175" s="40"/>
-      <c r="AA175" s="40"/>
-      <c r="AB175" s="40"/>
-      <c r="AC175" s="40"/>
+      <c r="Z175" s="23"/>
+      <c r="AA175" s="23"/>
+      <c r="AB175" s="23"/>
+      <c r="AC175" s="23"/>
       <c r="AD175" s="40"/>
       <c r="AF175" s="40"/>
     </row>
     <row r="176" spans="1:43" s="21" customFormat="1">
-      <c r="P176" s="22"/>
       <c r="Q176" s="23"/>
       <c r="R176" s="23"/>
       <c r="S176" s="23"/>
@@ -21660,6 +21756,7 @@
       <c r="AF176" s="40"/>
     </row>
     <row r="177" spans="9:32" s="21" customFormat="1">
+      <c r="P177" s="22"/>
       <c r="Q177" s="23"/>
       <c r="R177" s="23"/>
       <c r="S177" s="23"/>
@@ -21669,10 +21766,10 @@
       <c r="W177" s="23"/>
       <c r="X177" s="40"/>
       <c r="Y177" s="40"/>
-      <c r="Z177" s="23"/>
-      <c r="AA177" s="23"/>
-      <c r="AB177" s="23"/>
-      <c r="AC177" s="23"/>
+      <c r="Z177" s="40"/>
+      <c r="AA177" s="40"/>
+      <c r="AB177" s="40"/>
+      <c r="AC177" s="40"/>
       <c r="AD177" s="40"/>
       <c r="AF177" s="40"/>
     </row>
@@ -21687,28 +21784,27 @@
       <c r="W178" s="23"/>
       <c r="X178" s="40"/>
       <c r="Y178" s="40"/>
-      <c r="Z178" s="40"/>
-      <c r="AA178" s="40"/>
-      <c r="AB178" s="40"/>
-      <c r="AC178" s="40"/>
+      <c r="Z178" s="23"/>
+      <c r="AA178" s="23"/>
+      <c r="AB178" s="23"/>
+      <c r="AC178" s="23"/>
       <c r="AD178" s="40"/>
       <c r="AF178" s="40"/>
     </row>
     <row r="179" spans="9:32" s="21" customFormat="1">
-      <c r="P179" s="22"/>
       <c r="Q179" s="23"/>
       <c r="R179" s="23"/>
       <c r="S179" s="23"/>
       <c r="T179" s="23"/>
       <c r="U179" s="23"/>
       <c r="V179" s="23"/>
-      <c r="W179" s="23"/>
+      <c r="W179" s="40"/>
       <c r="X179" s="40"/>
       <c r="Y179" s="40"/>
-      <c r="Z179" s="23"/>
-      <c r="AA179" s="23"/>
-      <c r="AB179" s="23"/>
-      <c r="AC179" s="23"/>
+      <c r="Z179" s="40"/>
+      <c r="AA179" s="40"/>
+      <c r="AB179" s="40"/>
+      <c r="AC179" s="40"/>
       <c r="AD179" s="40"/>
       <c r="AF179" s="40"/>
     </row>
@@ -21719,30 +21815,31 @@
       <c r="T180" s="23"/>
       <c r="U180" s="23"/>
       <c r="V180" s="23"/>
-      <c r="W180" s="40"/>
+      <c r="W180" s="23"/>
       <c r="X180" s="40"/>
       <c r="Y180" s="40"/>
-      <c r="Z180" s="40"/>
-      <c r="AA180" s="40"/>
-      <c r="AB180" s="40"/>
-      <c r="AC180" s="40"/>
+      <c r="Z180" s="23"/>
+      <c r="AA180" s="23"/>
+      <c r="AB180" s="23"/>
+      <c r="AC180" s="23"/>
       <c r="AD180" s="40"/>
       <c r="AF180" s="40"/>
     </row>
     <row r="181" spans="9:32" s="21" customFormat="1">
+      <c r="P181" s="22"/>
       <c r="Q181" s="23"/>
       <c r="R181" s="23"/>
       <c r="S181" s="23"/>
       <c r="T181" s="23"/>
       <c r="U181" s="23"/>
       <c r="V181" s="23"/>
-      <c r="W181" s="23"/>
+      <c r="W181" s="40"/>
       <c r="X181" s="40"/>
       <c r="Y181" s="40"/>
-      <c r="Z181" s="23"/>
-      <c r="AA181" s="23"/>
-      <c r="AB181" s="23"/>
-      <c r="AC181" s="23"/>
+      <c r="Z181" s="40"/>
+      <c r="AA181" s="40"/>
+      <c r="AB181" s="40"/>
+      <c r="AC181" s="40"/>
       <c r="AD181" s="40"/>
       <c r="AF181" s="40"/>
     </row>
@@ -21790,17 +21887,35 @@
       <c r="T184" s="23"/>
       <c r="U184" s="23"/>
       <c r="V184" s="23"/>
-      <c r="W184" s="40"/>
+      <c r="W184" s="23"/>
       <c r="X184" s="40"/>
       <c r="Y184" s="40"/>
-      <c r="Z184" s="40"/>
-      <c r="AA184" s="40"/>
-      <c r="AB184" s="40"/>
-      <c r="AC184" s="40"/>
-      <c r="AD184" s="40"/>
+      <c r="Z184" s="23"/>
+      <c r="AA184" s="23"/>
+      <c r="AB184" s="23"/>
+      <c r="AC184" s="23"/>
+      <c r="AD184" s="23"/>
       <c r="AF184" s="40"/>
     </row>
     <row r="185" spans="9:32" s="21" customFormat="1">
+      <c r="I185" s="21">
+        <v>0</v>
+      </c>
+      <c r="J185" s="21">
+        <v>3</v>
+      </c>
+      <c r="K185" s="21">
+        <v>7</v>
+      </c>
+      <c r="L185" s="21">
+        <v>8</v>
+      </c>
+      <c r="M185" s="21">
+        <v>15</v>
+      </c>
+      <c r="N185" s="21">
+        <v>18</v>
+      </c>
       <c r="P185" s="22"/>
       <c r="Q185" s="23"/>
       <c r="R185" s="23"/>
@@ -21811,32 +21926,68 @@
       <c r="W185" s="23"/>
       <c r="X185" s="40"/>
       <c r="Y185" s="40"/>
-      <c r="Z185" s="23"/>
-      <c r="AA185" s="23"/>
+      <c r="Z185" s="40"/>
+      <c r="AA185" s="40"/>
       <c r="AB185" s="23"/>
       <c r="AC185" s="23"/>
       <c r="AD185" s="23"/>
       <c r="AF185" s="40"/>
     </row>
     <row r="186" spans="9:32" s="21" customFormat="1">
+      <c r="I186" s="21">
+        <v>0</v>
+      </c>
+      <c r="J186" s="21">
+        <v>1</v>
+      </c>
+      <c r="K186" s="21">
+        <v>3</v>
+      </c>
+      <c r="L186" s="21">
+        <v>7</v>
+      </c>
+      <c r="M186" s="21">
+        <v>8</v>
+      </c>
+      <c r="N186" s="21">
+        <v>18</v>
+      </c>
       <c r="P186" s="22"/>
-      <c r="Q186" s="23"/>
-      <c r="R186" s="23"/>
-      <c r="S186" s="23"/>
-      <c r="T186" s="23"/>
-      <c r="U186" s="23"/>
-      <c r="V186" s="23"/>
-      <c r="W186" s="23"/>
-      <c r="X186" s="40"/>
-      <c r="Y186" s="40"/>
-      <c r="Z186" s="40"/>
-      <c r="AA186" s="40"/>
-      <c r="AB186" s="23"/>
-      <c r="AC186" s="23"/>
-      <c r="AD186" s="23"/>
+      <c r="Q186" s="20"/>
+      <c r="R186" s="20"/>
+      <c r="S186" s="20"/>
+      <c r="T186" s="20"/>
+      <c r="U186" s="20"/>
+      <c r="V186" s="20"/>
+      <c r="W186" s="20"/>
+      <c r="X186" s="20"/>
+      <c r="Y186" s="20"/>
+      <c r="Z186" s="20"/>
+      <c r="AA186" s="20"/>
+      <c r="AB186" s="20"/>
+      <c r="AC186" s="20"/>
+      <c r="AD186" s="20"/>
       <c r="AF186" s="40"/>
     </row>
     <row r="187" spans="9:32" s="21" customFormat="1">
+      <c r="I187" s="21">
+        <v>0</v>
+      </c>
+      <c r="J187" s="21">
+        <v>1</v>
+      </c>
+      <c r="K187" s="21">
+        <v>5</v>
+      </c>
+      <c r="L187" s="21">
+        <v>5</v>
+      </c>
+      <c r="M187" s="21">
+        <v>6</v>
+      </c>
+      <c r="N187" s="21">
+        <v>18</v>
+      </c>
       <c r="P187" s="22"/>
       <c r="Q187" s="20"/>
       <c r="R187" s="20"/>
@@ -21844,14 +21995,14 @@
       <c r="T187" s="20"/>
       <c r="U187" s="20"/>
       <c r="V187" s="20"/>
-      <c r="W187" s="20"/>
-      <c r="X187" s="20"/>
+      <c r="W187" s="15"/>
+      <c r="X187" s="15"/>
       <c r="Y187" s="20"/>
       <c r="Z187" s="20"/>
       <c r="AA187" s="20"/>
       <c r="AB187" s="20"/>
       <c r="AC187" s="20"/>
-      <c r="AD187" s="20"/>
+      <c r="AD187" s="15"/>
       <c r="AF187" s="40"/>
     </row>
     <row r="188" spans="9:32" s="21" customFormat="1">
@@ -21873,24 +22024,6 @@
       <c r="AF188" s="40"/>
     </row>
     <row r="189" spans="9:32" s="21" customFormat="1">
-      <c r="I189" s="21">
-        <v>2</v>
-      </c>
-      <c r="J189" s="21">
-        <v>2</v>
-      </c>
-      <c r="K189" s="21">
-        <v>3</v>
-      </c>
-      <c r="L189" s="21">
-        <v>5</v>
-      </c>
-      <c r="M189" s="21">
-        <v>14</v>
-      </c>
-      <c r="N189" s="21">
-        <v>17</v>
-      </c>
       <c r="P189" s="22"/>
       <c r="Q189" s="23"/>
       <c r="R189" s="23"/>
@@ -21909,24 +22042,6 @@
       <c r="AF189" s="40"/>
     </row>
     <row r="190" spans="9:32" s="21" customFormat="1">
-      <c r="I190" s="21">
-        <v>0</v>
-      </c>
-      <c r="J190" s="21">
-        <v>1</v>
-      </c>
-      <c r="K190" s="21">
-        <v>2</v>
-      </c>
-      <c r="L190" s="21">
-        <v>6</v>
-      </c>
-      <c r="M190" s="21">
-        <v>6</v>
-      </c>
-      <c r="N190" s="21">
-        <v>17</v>
-      </c>
       <c r="P190" s="22"/>
       <c r="Q190" s="20"/>
       <c r="R190" s="20"/>
@@ -21945,24 +22060,6 @@
       <c r="AF190" s="40"/>
     </row>
     <row r="191" spans="9:32" s="21" customFormat="1">
-      <c r="I191" s="21">
-        <v>0</v>
-      </c>
-      <c r="J191" s="21">
-        <v>2</v>
-      </c>
-      <c r="K191" s="21">
-        <v>2</v>
-      </c>
-      <c r="L191" s="21">
-        <v>4</v>
-      </c>
-      <c r="M191" s="21">
-        <v>11</v>
-      </c>
-      <c r="N191" s="21">
-        <v>17</v>
-      </c>
       <c r="P191" s="22"/>
       <c r="Q191" s="23"/>
       <c r="R191" s="23"/>
@@ -21981,24 +22078,6 @@
       <c r="AF191" s="40"/>
     </row>
     <row r="192" spans="9:32" s="21" customFormat="1">
-      <c r="I192" s="21">
-        <v>0</v>
-      </c>
-      <c r="J192" s="21">
-        <v>2</v>
-      </c>
-      <c r="K192" s="21">
-        <v>2</v>
-      </c>
-      <c r="L192" s="21">
-        <v>4</v>
-      </c>
-      <c r="M192" s="21">
-        <v>6</v>
-      </c>
-      <c r="N192" s="21">
-        <v>17</v>
-      </c>
       <c r="P192" s="22"/>
       <c r="Q192" s="23"/>
       <c r="R192" s="23"/>
@@ -22016,25 +22095,7 @@
       <c r="AD192" s="40"/>
       <c r="AF192" s="40"/>
     </row>
-    <row r="193" spans="9:32" s="21" customFormat="1">
-      <c r="I193" s="21">
-        <v>0</v>
-      </c>
-      <c r="J193" s="21">
-        <v>1</v>
-      </c>
-      <c r="K193" s="21">
-        <v>1</v>
-      </c>
-      <c r="L193" s="21">
-        <v>2</v>
-      </c>
-      <c r="M193" s="21">
-        <v>3</v>
-      </c>
-      <c r="N193" s="21">
-        <v>14</v>
-      </c>
+    <row r="193" spans="16:32" s="21" customFormat="1">
       <c r="P193" s="22"/>
       <c r="Q193" s="20"/>
       <c r="R193" s="20"/>
@@ -22052,25 +22113,7 @@
       <c r="AD193" s="20"/>
       <c r="AF193" s="40"/>
     </row>
-    <row r="194" spans="9:32" s="21" customFormat="1">
-      <c r="I194" s="21">
-        <v>0</v>
-      </c>
-      <c r="J194" s="21">
-        <v>1</v>
-      </c>
-      <c r="K194" s="21">
-        <v>2</v>
-      </c>
-      <c r="L194" s="21">
-        <v>3</v>
-      </c>
-      <c r="M194" s="21">
-        <v>3</v>
-      </c>
-      <c r="N194" s="21">
-        <v>14</v>
-      </c>
+    <row r="194" spans="16:32" s="21" customFormat="1">
       <c r="P194" s="22"/>
       <c r="Q194" s="20"/>
       <c r="R194" s="20"/>
@@ -22088,25 +22131,7 @@
       <c r="AD194" s="20"/>
       <c r="AF194" s="40"/>
     </row>
-    <row r="195" spans="9:32" s="21" customFormat="1">
-      <c r="I195" s="21">
-        <v>0</v>
-      </c>
-      <c r="J195" s="21">
-        <v>1</v>
-      </c>
-      <c r="K195" s="21">
-        <v>1</v>
-      </c>
-      <c r="L195" s="21">
-        <v>3</v>
-      </c>
-      <c r="M195" s="21">
-        <v>5</v>
-      </c>
-      <c r="N195" s="21">
-        <v>6</v>
-      </c>
+    <row r="195" spans="16:32" s="21" customFormat="1">
       <c r="P195" s="22"/>
       <c r="Q195" s="20"/>
       <c r="R195" s="20"/>
@@ -22124,7 +22149,7 @@
       <c r="AD195" s="15"/>
       <c r="AF195" s="40"/>
     </row>
-    <row r="196" spans="9:32" s="21" customFormat="1">
+    <row r="196" spans="16:32" s="21" customFormat="1">
       <c r="P196" s="22"/>
       <c r="Q196" s="20"/>
       <c r="R196" s="20"/>
@@ -22142,7 +22167,7 @@
       <c r="AD196" s="15"/>
       <c r="AF196" s="40"/>
     </row>
-    <row r="197" spans="9:32" s="21" customFormat="1">
+    <row r="197" spans="16:32" s="21" customFormat="1">
       <c r="P197" s="22"/>
       <c r="Q197" s="23"/>
       <c r="R197" s="23"/>
@@ -22160,7 +22185,7 @@
       <c r="AD197" s="40"/>
       <c r="AF197" s="40"/>
     </row>
-    <row r="198" spans="9:32" s="21" customFormat="1">
+    <row r="198" spans="16:32" s="21" customFormat="1">
       <c r="P198" s="22"/>
       <c r="Q198" s="23"/>
       <c r="R198" s="23"/>
@@ -22178,7 +22203,7 @@
       <c r="AD198" s="40"/>
       <c r="AF198" s="40"/>
     </row>
-    <row r="199" spans="9:32" s="21" customFormat="1">
+    <row r="199" spans="16:32" s="21" customFormat="1">
       <c r="P199" s="22"/>
       <c r="Q199" s="23"/>
       <c r="R199" s="23"/>
@@ -22196,7 +22221,7 @@
       <c r="AD199" s="40"/>
       <c r="AF199" s="40"/>
     </row>
-    <row r="200" spans="9:32" s="21" customFormat="1">
+    <row r="200" spans="16:32" s="21" customFormat="1">
       <c r="Q200" s="23"/>
       <c r="R200" s="23"/>
       <c r="S200" s="23"/>
@@ -22213,7 +22238,7 @@
       <c r="AD200" s="40"/>
       <c r="AF200" s="40"/>
     </row>
-    <row r="201" spans="9:32" s="21" customFormat="1">
+    <row r="201" spans="16:32" s="21" customFormat="1">
       <c r="P201" s="22"/>
       <c r="Q201" s="23"/>
       <c r="R201" s="23"/>
@@ -22231,7 +22256,7 @@
       <c r="AD201" s="40"/>
       <c r="AF201" s="40"/>
     </row>
-    <row r="202" spans="9:32" s="21" customFormat="1">
+    <row r="202" spans="16:32" s="21" customFormat="1">
       <c r="Q202" s="23"/>
       <c r="R202" s="23"/>
       <c r="S202" s="23"/>
@@ -22248,7 +22273,7 @@
       <c r="AD202" s="40"/>
       <c r="AF202" s="40"/>
     </row>
-    <row r="203" spans="9:32" s="21" customFormat="1">
+    <row r="203" spans="16:32" s="21" customFormat="1">
       <c r="Q203" s="23"/>
       <c r="R203" s="23"/>
       <c r="S203" s="23"/>
@@ -22265,7 +22290,7 @@
       <c r="AD203" s="40"/>
       <c r="AF203" s="40"/>
     </row>
-    <row r="204" spans="9:32" s="21" customFormat="1">
+    <row r="204" spans="16:32" s="21" customFormat="1">
       <c r="P204" s="22"/>
       <c r="Q204" s="23"/>
       <c r="R204" s="23"/>
@@ -22283,7 +22308,7 @@
       <c r="AD204" s="40"/>
       <c r="AF204" s="40"/>
     </row>
-    <row r="205" spans="9:32" s="21" customFormat="1">
+    <row r="205" spans="16:32" s="21" customFormat="1">
       <c r="Q205" s="23"/>
       <c r="R205" s="23"/>
       <c r="S205" s="23"/>
@@ -22300,7 +22325,7 @@
       <c r="AD205" s="40"/>
       <c r="AF205" s="40"/>
     </row>
-    <row r="206" spans="9:32" s="21" customFormat="1">
+    <row r="206" spans="16:32" s="21" customFormat="1">
       <c r="P206" s="22"/>
       <c r="Q206" s="23"/>
       <c r="R206" s="23"/>
@@ -22318,7 +22343,7 @@
       <c r="AD206" s="40"/>
       <c r="AF206" s="40"/>
     </row>
-    <row r="207" spans="9:32" s="21" customFormat="1">
+    <row r="207" spans="16:32" s="21" customFormat="1">
       <c r="P207" s="22"/>
       <c r="Q207" s="23"/>
       <c r="R207" s="23"/>
@@ -22336,7 +22361,7 @@
       <c r="AD207" s="40"/>
       <c r="AF207" s="40"/>
     </row>
-    <row r="208" spans="9:32" s="21" customFormat="1">
+    <row r="208" spans="16:32" s="21" customFormat="1">
       <c r="P208" s="22"/>
       <c r="Q208" s="23"/>
       <c r="R208" s="23"/>
@@ -34082,10 +34107,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO235"/>
+  <dimension ref="A1:AO236"/>
   <sheetViews>
     <sheetView topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G171" sqref="G171"/>
+      <selection activeCell="H173" sqref="H173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -37555,12 +37580,24 @@
       </c>
     </row>
     <row r="166" spans="1:18">
-      <c r="A166" s="10"/>
-      <c r="B166" s="10"/>
-      <c r="C166" s="10"/>
+      <c r="A166" s="9">
+        <v>1</v>
+      </c>
+      <c r="B166" s="9">
+        <v>1</v>
+      </c>
+      <c r="C166" s="9">
+        <v>1</v>
+      </c>
       <c r="D166" s="10"/>
       <c r="E166" s="10"/>
       <c r="F166" s="10"/>
+      <c r="H166" s="11">
+        <v>2</v>
+      </c>
+      <c r="I166" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="167" spans="1:18">
       <c r="A167" s="10"/>
@@ -37569,6 +37606,7 @@
       <c r="D167" s="10"/>
       <c r="E167" s="10"/>
       <c r="F167" s="10"/>
+      <c r="I167" s="10"/>
     </row>
     <row r="168" spans="1:18">
       <c r="A168" s="10"/>
@@ -37914,11 +37952,13 @@
     </row>
     <row r="213" spans="1:6">
       <c r="A213" s="10"/>
+      <c r="B213" s="10"/>
       <c r="C213" s="10"/>
       <c r="D213" s="10"/>
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="10"/>
+      <c r="B214" s="10"/>
       <c r="C214" s="10"/>
       <c r="D214" s="10"/>
     </row>
@@ -37980,6 +38020,7 @@
     <row r="226" spans="1:4">
       <c r="A226" s="10"/>
       <c r="C226" s="10"/>
+      <c r="D226" s="10"/>
     </row>
     <row r="227" spans="1:4">
       <c r="A227" s="10"/>
@@ -37994,6 +38035,7 @@
       <c r="C229" s="10"/>
     </row>
     <row r="230" spans="1:4">
+      <c r="A230" s="10"/>
       <c r="C230" s="10"/>
     </row>
     <row r="231" spans="1:4">
@@ -38010,6 +38052,9 @@
     </row>
     <row r="235" spans="1:4">
       <c r="C235" s="10"/>
+    </row>
+    <row r="236" spans="1:4">
+      <c r="C236" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -38023,7 +38068,7 @@
   <dimension ref="A1:U197"/>
   <sheetViews>
     <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="D172" sqref="D172"/>
+      <selection activeCell="L174" sqref="L174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -42103,18 +42148,54 @@
       </c>
     </row>
     <row r="166" spans="1:19" customFormat="1">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
-      <c r="C166" s="1"/>
+      <c r="A166" s="1">
+        <v>1</v>
+      </c>
+      <c r="B166" s="1">
+        <v>2</v>
+      </c>
+      <c r="C166" s="1">
+        <v>3</v>
+      </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
-      <c r="F166" s="18"/>
-      <c r="G166" s="18"/>
-      <c r="H166" s="18"/>
-      <c r="I166" s="18"/>
-      <c r="J166" s="18"/>
-      <c r="K166" s="18"/>
+      <c r="F166" s="18">
+        <v>1</v>
+      </c>
+      <c r="G166" s="18">
+        <v>0</v>
+      </c>
+      <c r="H166" s="18">
+        <v>3</v>
+      </c>
+      <c r="I166" s="18">
+        <v>0</v>
+      </c>
+      <c r="J166" s="18">
+        <v>2</v>
+      </c>
+      <c r="K166" s="18">
+        <v>0</v>
+      </c>
       <c r="L166" s="18"/>
+      <c r="N166" s="1">
+        <v>0</v>
+      </c>
+      <c r="O166" s="1">
+        <v>2</v>
+      </c>
+      <c r="P166" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q166" s="1">
+        <v>3</v>
+      </c>
+      <c r="R166" s="1">
+        <v>4</v>
+      </c>
+      <c r="S166" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="167" spans="1:19" customFormat="1">
       <c r="A167" s="1"/>
@@ -42177,10 +42258,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A100:AN165"/>
+  <dimension ref="A100:AN167"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="R168" sqref="R168"/>
+    <sheetView topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="H175" sqref="H175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -45232,6 +45313,48 @@
         <v>2</v>
       </c>
     </row>
+    <row r="166" spans="1:19">
+      <c r="A166" s="11">
+        <v>3</v>
+      </c>
+      <c r="B166" s="10"/>
+      <c r="C166" s="10"/>
+      <c r="D166" s="9">
+        <v>1</v>
+      </c>
+      <c r="E166" s="10"/>
+      <c r="F166" s="10"/>
+      <c r="H166" s="9">
+        <v>1</v>
+      </c>
+      <c r="I166" s="9">
+        <v>1</v>
+      </c>
+      <c r="L166" s="16">
+        <v>1</v>
+      </c>
+      <c r="M166" s="16">
+        <v>1</v>
+      </c>
+      <c r="N166" s="16">
+        <v>1</v>
+      </c>
+      <c r="O166" s="16">
+        <v>4</v>
+      </c>
+      <c r="P166" s="16">
+        <v>8</v>
+      </c>
+      <c r="Q166" s="16">
+        <v>9</v>
+      </c>
+      <c r="S166" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="167" spans="1:19">
+      <c r="D167" s="10"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45244,7 +45367,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -45468,7 +45591,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="18">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" s="18">
         <v>15</v>
@@ -45603,10 +45726,10 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="19">
         <v>6</v>
@@ -45642,7 +45765,7 @@
         <v>4</v>
       </c>
       <c r="O8" s="18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P8" s="18">
         <v>0</v>
@@ -45668,7 +45791,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="18">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K9" s="18">
         <v>12</v>
@@ -45677,7 +45800,7 @@
         <v>2</v>
       </c>
       <c r="M9" s="18">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="N9" s="18">
         <v>28</v>
@@ -45699,6 +45822,9 @@
       <c r="G10" s="18">
         <v>2</v>
       </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
       <c r="I10" s="18">
         <v>5</v>
       </c>
@@ -45712,7 +45838,7 @@
         <v>1</v>
       </c>
       <c r="P10" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -45720,13 +45846,13 @@
         <v>35</v>
       </c>
       <c r="E11" s="18">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F11" s="19">
         <v>11</v>
       </c>
       <c r="G11" s="18">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I11" s="18">
         <v>11</v>
@@ -45743,7 +45869,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="C12" s="19">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F12" s="19">
         <v>9</v>
@@ -45755,7 +45881,7 @@
         <v>5</v>
       </c>
       <c r="L12" s="18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N12" s="18">
         <v>17</v>
@@ -45766,7 +45892,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="18">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K13" s="18">
         <v>14</v>
@@ -45780,15 +45906,15 @@
         <v>29</v>
       </c>
       <c r="K14" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N14" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="F15" s="19">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cp: add d3  nad cpup
</commit_message>
<xml_diff>
--- a/demos/cp/cp.xlsx
+++ b/demos/cp/cp.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId7"/>
     <sheet name="Sheet7" sheetId="9" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -112,6 +113,10 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -881,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO104"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF71" sqref="AF71"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -5601,7 +5606,7 @@
         <v>3</v>
       </c>
       <c r="P47" s="7">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Q47" s="7">
         <v>7</v>
@@ -5729,7 +5734,7 @@
       <c r="Y48" s="7">
         <v>0</v>
       </c>
-      <c r="Z48" s="7">
+      <c r="Z48" s="25">
         <v>13</v>
       </c>
       <c r="AA48" s="7">
@@ -5828,7 +5833,7 @@
       <c r="Y49" s="7">
         <v>2</v>
       </c>
-      <c r="Z49" s="7">
+      <c r="Z49" s="25">
         <v>4</v>
       </c>
       <c r="AA49" s="7">
@@ -5927,7 +5932,7 @@
       <c r="Y50" s="7">
         <v>3</v>
       </c>
-      <c r="Z50" s="7">
+      <c r="Z50" s="25">
         <v>0</v>
       </c>
       <c r="AA50" s="7">
@@ -6376,7 +6381,9 @@
       <c r="I55" s="7">
         <v>13</v>
       </c>
-      <c r="J55" s="7"/>
+      <c r="J55" s="7">
+        <v>1</v>
+      </c>
       <c r="K55" s="7">
         <v>2</v>
       </c>
@@ -6447,7 +6454,7 @@
     </row>
     <row r="56" spans="1:33" s="25" customFormat="1">
       <c r="A56" s="7">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B56" s="7">
         <v>0</v>
@@ -6475,7 +6482,7 @@
       </c>
       <c r="J56" s="7"/>
       <c r="K56" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L56" s="7">
         <v>6</v>
@@ -6509,7 +6516,7 @@
         <v>5</v>
       </c>
       <c r="W56" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X56" s="7">
         <v>3</v>
@@ -6620,10 +6627,10 @@
         <v>1</v>
       </c>
       <c r="AD57" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AE57" s="7">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AF57" s="7">
         <v>2</v>
@@ -6677,7 +6684,7 @@
         <v>0</v>
       </c>
       <c r="R58" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S58" s="7">
         <v>3</v>
@@ -6724,7 +6731,7 @@
         <v>4</v>
       </c>
       <c r="C59" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D59" s="7">
         <v>6</v>
@@ -6735,7 +6742,7 @@
       <c r="F59" s="7">
         <v>8</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="25">
         <v>4</v>
       </c>
       <c r="H59" s="7">
@@ -6811,7 +6818,7 @@
       <c r="F60" s="7">
         <v>2</v>
       </c>
-      <c r="G60" s="7">
+      <c r="G60" s="25">
         <v>9</v>
       </c>
       <c r="H60" s="7">
@@ -6839,7 +6846,7 @@
         <v>3</v>
       </c>
       <c r="T60" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U60" s="7">
         <v>1</v>
@@ -6869,7 +6876,7 @@
         <v>3</v>
       </c>
       <c r="AG60" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:33" s="14" customFormat="1">
@@ -6887,11 +6894,11 @@
       <c r="F61" s="7">
         <v>3</v>
       </c>
-      <c r="G61" s="7">
+      <c r="G61" s="25">
         <v>5</v>
       </c>
       <c r="H61" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I61" s="7">
         <v>0</v>
@@ -6936,7 +6943,7 @@
         <v>8</v>
       </c>
       <c r="AA61" s="7">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AB61" s="7">
         <v>12</v>
@@ -6975,13 +6982,13 @@
       <c r="J62" s="3"/>
       <c r="K62" s="7"/>
       <c r="L62" s="7">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M62" s="7">
         <v>4</v>
       </c>
       <c r="N62" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O62" s="7">
         <v>4</v>
@@ -7016,7 +7023,7 @@
         <v>12</v>
       </c>
       <c r="AC62" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD62" s="7"/>
       <c r="AE62" s="3"/>
@@ -7045,7 +7052,7 @@
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
@@ -7066,7 +7073,9 @@
         <v>1</v>
       </c>
       <c r="T63" s="3"/>
-      <c r="U63" s="4"/>
+      <c r="U63" s="4">
+        <v>0</v>
+      </c>
       <c r="V63" s="4">
         <v>0</v>
       </c>
@@ -7075,7 +7084,7 @@
         <v>3</v>
       </c>
       <c r="Y63" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z63" s="4">
         <v>12</v>
@@ -7087,7 +7096,7 @@
       <c r="AD63" s="7"/>
       <c r="AE63" s="3"/>
       <c r="AF63" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AG63" s="5"/>
     </row>
@@ -7108,7 +7117,9 @@
         <v>0</v>
       </c>
       <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
+      <c r="I64" s="4">
+        <v>0</v>
+      </c>
       <c r="K64" s="3"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4">
@@ -7127,7 +7138,9 @@
         <v>0</v>
       </c>
       <c r="T64" s="7"/>
-      <c r="U64" s="38"/>
+      <c r="U64" s="40">
+        <v>0</v>
+      </c>
       <c r="V64" s="4">
         <v>4</v>
       </c>
@@ -7149,7 +7162,7 @@
     </row>
     <row r="65" spans="1:33">
       <c r="B65" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="7">
@@ -7158,7 +7171,9 @@
       <c r="E65" s="4">
         <v>0</v>
       </c>
-      <c r="F65" s="7"/>
+      <c r="F65" s="7">
+        <v>1</v>
+      </c>
       <c r="G65" s="2">
         <v>4</v>
       </c>
@@ -7210,6 +7225,9 @@
         <v>2</v>
       </c>
       <c r="F66" s="4"/>
+      <c r="G66" s="2">
+        <v>0</v>
+      </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
       <c r="J66" s="3"/>
@@ -7226,7 +7244,7 @@
       </c>
       <c r="R66" s="4"/>
       <c r="S66" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T66" s="3"/>
       <c r="U66" s="4"/>
@@ -7242,7 +7260,7 @@
         <v>4</v>
       </c>
       <c r="AB66" s="14">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="AD66" s="4"/>
       <c r="AE66" s="3"/>
@@ -7257,6 +7275,9 @@
         <v>17</v>
       </c>
       <c r="F67" s="4"/>
+      <c r="G67" s="2">
+        <v>0</v>
+      </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="K67" s="3"/>
@@ -7266,7 +7287,7 @@
       </c>
       <c r="N67" s="4"/>
       <c r="O67" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P67" s="4"/>
       <c r="Q67" s="4">
@@ -7281,9 +7302,11 @@
       </c>
       <c r="W67" s="4"/>
       <c r="X67" s="4">
-        <v>1</v>
-      </c>
-      <c r="Z67" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="Z67" s="4">
+        <v>1</v>
+      </c>
       <c r="AB67" s="12"/>
       <c r="AD67" s="4"/>
       <c r="AE67" s="3"/>
@@ -7315,7 +7338,7 @@
       <c r="T68" s="3"/>
       <c r="U68" s="4"/>
       <c r="V68" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W68" s="4"/>
       <c r="X68" s="4"/>
@@ -7350,7 +7373,9 @@
       <c r="S69" s="4"/>
       <c r="T69" s="3"/>
       <c r="U69" s="4"/>
-      <c r="V69" s="4"/>
+      <c r="V69" s="4">
+        <v>0</v>
+      </c>
       <c r="W69" s="4"/>
       <c r="X69" s="4"/>
       <c r="Z69" s="4"/>
@@ -7366,7 +7391,7 @@
         <v>1</v>
       </c>
       <c r="E70" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F70" s="7"/>
       <c r="H70" s="4"/>
@@ -7440,13 +7465,13 @@
       <c r="J72" s="3"/>
       <c r="L72" s="4"/>
       <c r="M72" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N72" s="4"/>
       <c r="O72" s="4"/>
       <c r="P72" s="4"/>
       <c r="Q72" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R72" s="4"/>
       <c r="S72" s="4"/>
@@ -7470,11 +7495,15 @@
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
       <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
+      <c r="M73" s="4">
+        <v>0</v>
+      </c>
       <c r="N73" s="4"/>
       <c r="O73" s="4"/>
       <c r="P73" s="4"/>
-      <c r="Q73" s="4"/>
+      <c r="Q73" s="4">
+        <v>0</v>
+      </c>
       <c r="R73" s="4"/>
       <c r="S73" s="4"/>
       <c r="T73" s="3"/>
@@ -7521,7 +7550,9 @@
     <row r="75" spans="1:33">
       <c r="A75" s="5"/>
       <c r="C75" s="5"/>
-      <c r="D75" s="3"/>
+      <c r="D75" s="3">
+        <v>1</v>
+      </c>
       <c r="F75" s="4"/>
       <c r="H75" s="4"/>
       <c r="J75" s="3"/>
@@ -8013,8 +8044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT961"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H181" sqref="H181"/>
+    <sheetView topLeftCell="A154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I183" sqref="I183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5"/>
@@ -21080,7 +21111,7 @@
         <v>1</v>
       </c>
       <c r="V160" s="20">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W160" s="20"/>
       <c r="X160" s="19">
@@ -21174,7 +21205,7 @@
         <v>3</v>
       </c>
       <c r="S161" s="20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="T161" s="19">
         <v>0</v>
@@ -21183,7 +21214,7 @@
         <v>10</v>
       </c>
       <c r="V161" s="20">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="W161" s="20"/>
       <c r="X161" s="19">
@@ -21272,7 +21303,7 @@
         <v>2</v>
       </c>
       <c r="S162" s="20">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="T162" s="19">
         <v>2</v>
@@ -21480,7 +21511,7 @@
         <v>8</v>
       </c>
       <c r="U164" s="20">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="V164" s="19">
         <v>4</v>
@@ -21492,17 +21523,19 @@
       <c r="Y164" s="19">
         <v>2</v>
       </c>
-      <c r="Z164" s="22">
-        <v>4</v>
-      </c>
-      <c r="AA164" s="22">
-        <v>5</v>
-      </c>
-      <c r="AB164" s="22">
+      <c r="Z164" s="19">
+        <v>4</v>
+      </c>
+      <c r="AA164" s="19">
+        <v>5</v>
+      </c>
+      <c r="AB164" s="19">
         <v>8</v>
       </c>
       <c r="AC164" s="20"/>
-      <c r="AD164" s="20"/>
+      <c r="AD164" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="AF164" s="39"/>
       <c r="AH164" s="21">
         <v>0</v>
@@ -21667,7 +21700,7 @@
       </c>
       <c r="P166" s="22"/>
       <c r="Q166" s="20">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="R166" s="19">
         <v>8</v>
@@ -21701,7 +21734,9 @@
         <v>8</v>
       </c>
       <c r="AC166" s="20"/>
-      <c r="AD166" s="20"/>
+      <c r="AD166" s="20" t="s">
+        <v>23</v>
+      </c>
       <c r="AF166" s="39"/>
       <c r="AH166" s="21">
         <v>0</v>
@@ -21767,7 +21802,7 @@
       </c>
       <c r="P167" s="22"/>
       <c r="Q167" s="23">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="R167" s="22">
         <v>0</v>
@@ -21801,7 +21836,9 @@
         <v>5</v>
       </c>
       <c r="AC167" s="23"/>
-      <c r="AD167" s="23"/>
+      <c r="AD167" s="23" t="s">
+        <v>23</v>
+      </c>
       <c r="AF167" s="39"/>
       <c r="AH167" s="21">
         <v>0</v>
@@ -21975,7 +22012,7 @@
         <v>0</v>
       </c>
       <c r="R169" s="23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S169" s="22">
         <v>3</v>
@@ -21984,7 +22021,7 @@
         <v>2</v>
       </c>
       <c r="U169" s="23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V169" s="22">
         <v>2</v>
@@ -22004,7 +22041,9 @@
       </c>
       <c r="AB169" s="23"/>
       <c r="AC169" s="23"/>
-      <c r="AD169" s="23"/>
+      <c r="AD169" s="23" t="s">
+        <v>23</v>
+      </c>
       <c r="AF169" s="39"/>
       <c r="AH169" s="21">
         <v>0</v>
@@ -22076,7 +22115,7 @@
         <v>2</v>
       </c>
       <c r="R170" s="23">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="S170" s="22">
         <v>0</v>
@@ -22107,7 +22146,9 @@
         <v>3</v>
       </c>
       <c r="AC170" s="23"/>
-      <c r="AD170" s="23"/>
+      <c r="AD170" s="23" t="s">
+        <v>23</v>
+      </c>
       <c r="AF170" s="39"/>
       <c r="AH170" s="21">
         <v>0</v>
@@ -22172,13 +22213,13 @@
         <v>20</v>
       </c>
       <c r="P171" s="22"/>
-      <c r="Q171" s="20">
-        <v>4</v>
-      </c>
-      <c r="R171" s="20">
-        <v>4</v>
-      </c>
-      <c r="S171" s="20">
+      <c r="Q171" s="19">
+        <v>4</v>
+      </c>
+      <c r="R171" s="19">
+        <v>4</v>
+      </c>
+      <c r="S171" s="19">
         <v>4</v>
       </c>
       <c r="T171" s="19">
@@ -22187,7 +22228,7 @@
       <c r="U171" s="19">
         <v>2</v>
       </c>
-      <c r="V171" s="20">
+      <c r="V171" s="19">
         <v>4</v>
       </c>
       <c r="W171" s="20"/>
@@ -22197,10 +22238,18 @@
       <c r="Y171" s="19">
         <v>2</v>
       </c>
-      <c r="Z171" s="20"/>
-      <c r="AA171" s="20"/>
-      <c r="AB171" s="20"/>
-      <c r="AC171" s="20"/>
+      <c r="Z171" s="19">
+        <v>4</v>
+      </c>
+      <c r="AA171" s="19">
+        <v>4</v>
+      </c>
+      <c r="AB171" s="19">
+        <v>4</v>
+      </c>
+      <c r="AC171" s="19">
+        <v>4</v>
+      </c>
       <c r="AD171" s="20"/>
       <c r="AF171" s="39"/>
       <c r="AH171" s="21">
@@ -22266,23 +22315,23 @@
         <v>10</v>
       </c>
       <c r="P172" s="22"/>
-      <c r="Q172" s="23">
-        <v>3</v>
+      <c r="Q172" s="22">
+        <v>4</v>
       </c>
       <c r="R172" s="22">
         <v>1</v>
       </c>
       <c r="S172" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T172" s="22">
         <v>0</v>
       </c>
       <c r="U172" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V172" s="23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W172" s="23"/>
       <c r="X172" s="22">
@@ -22291,7 +22340,9 @@
       <c r="Y172" s="19">
         <v>1</v>
       </c>
-      <c r="Z172" s="23"/>
+      <c r="Z172" s="19">
+        <v>4</v>
+      </c>
       <c r="AA172" s="23"/>
       <c r="AB172" s="23"/>
       <c r="AC172" s="23"/>
@@ -22358,7 +22409,7 @@
       </c>
       <c r="P173" s="22"/>
       <c r="Q173" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R173" s="22">
         <v>1</v>
@@ -22367,12 +22418,12 @@
         <v>1</v>
       </c>
       <c r="T173" s="23">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U173" s="23">
-        <v>2</v>
-      </c>
-      <c r="V173" s="23">
+        <v>4</v>
+      </c>
+      <c r="V173" s="22">
         <v>2</v>
       </c>
       <c r="W173" s="23"/>
@@ -22382,7 +22433,9 @@
       <c r="Y173" s="22">
         <v>1</v>
       </c>
-      <c r="Z173" s="23"/>
+      <c r="Z173" s="19">
+        <v>2</v>
+      </c>
       <c r="AA173" s="23"/>
       <c r="AB173" s="23"/>
       <c r="AC173" s="23"/>
@@ -22454,29 +22507,31 @@
         <v>14</v>
       </c>
       <c r="P174" s="22"/>
-      <c r="Q174" s="23">
-        <v>1</v>
+      <c r="Q174" s="22">
+        <v>2</v>
       </c>
       <c r="R174" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S174" s="22">
         <v>0</v>
       </c>
       <c r="T174" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="U174" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="V174" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W174" s="23"/>
       <c r="X174" s="21">
         <v>0</v>
       </c>
-      <c r="Y174" s="39"/>
+      <c r="Y174" s="16">
+        <v>2</v>
+      </c>
       <c r="Z174" s="23"/>
       <c r="AA174" s="23"/>
       <c r="AB174" s="23"/>
@@ -22547,27 +22602,33 @@
       </c>
       <c r="P175" s="22"/>
       <c r="Q175" s="20">
-        <v>0</v>
-      </c>
-      <c r="R175" s="20">
+        <v>2</v>
+      </c>
+      <c r="R175" s="19">
         <v>0</v>
       </c>
       <c r="S175" s="20">
-        <v>0</v>
-      </c>
-      <c r="T175" s="20">
-        <v>0</v>
-      </c>
-      <c r="U175" s="20">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="T175" s="19">
+        <v>1</v>
+      </c>
+      <c r="U175" s="19">
+        <v>1</v>
       </c>
       <c r="V175" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W175" s="20"/>
-      <c r="X175" s="15"/>
-      <c r="Y175" s="15"/>
-      <c r="Z175" s="20"/>
+      <c r="X175" s="16">
+        <v>0</v>
+      </c>
+      <c r="Y175" s="16">
+        <v>1</v>
+      </c>
+      <c r="Z175" s="19">
+        <v>1</v>
+      </c>
       <c r="AA175" s="20"/>
       <c r="AB175" s="20"/>
       <c r="AC175" s="20"/>
@@ -22596,31 +22657,149 @@
       </c>
     </row>
     <row r="176" spans="1:43" s="21" customFormat="1">
+      <c r="A176" s="21">
+        <v>4</v>
+      </c>
+      <c r="B176" s="21">
+        <v>4</v>
+      </c>
+      <c r="C176" s="21">
+        <v>4</v>
+      </c>
+      <c r="D176" s="21">
+        <v>0</v>
+      </c>
+      <c r="E176" s="21">
+        <v>2</v>
+      </c>
+      <c r="F176" s="21">
+        <v>4</v>
+      </c>
+      <c r="I176" s="21">
+        <v>0</v>
+      </c>
+      <c r="J176" s="21">
+        <v>2</v>
+      </c>
+      <c r="K176" s="21">
+        <v>4</v>
+      </c>
+      <c r="L176" s="21">
+        <v>4</v>
+      </c>
+      <c r="M176" s="21">
+        <v>4</v>
+      </c>
+      <c r="N176" s="21">
+        <v>4</v>
+      </c>
       <c r="P176" s="22"/>
-      <c r="Q176" s="20"/>
-      <c r="R176" s="20"/>
-      <c r="S176" s="20"/>
-      <c r="T176" s="20"/>
-      <c r="U176" s="20"/>
-      <c r="V176" s="20"/>
+      <c r="Q176" s="20">
+        <v>1</v>
+      </c>
+      <c r="R176" s="20">
+        <v>1</v>
+      </c>
+      <c r="S176" s="19">
+        <v>0</v>
+      </c>
+      <c r="T176" s="20">
+        <v>1</v>
+      </c>
+      <c r="U176" s="19">
+        <v>0</v>
+      </c>
+      <c r="V176" s="20">
+        <v>1</v>
+      </c>
       <c r="W176" s="20"/>
-      <c r="X176" s="20"/>
-      <c r="Y176" s="20"/>
+      <c r="X176" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y176" s="19">
+        <v>0</v>
+      </c>
       <c r="Z176" s="20"/>
       <c r="AA176" s="20"/>
       <c r="AB176" s="20"/>
       <c r="AC176" s="20"/>
       <c r="AD176" s="20"/>
       <c r="AF176" s="39"/>
-    </row>
-    <row r="177" spans="16:32" s="21" customFormat="1">
+      <c r="AH176" s="21">
+        <v>0</v>
+      </c>
+      <c r="AI176" s="21">
+        <v>2</v>
+      </c>
+      <c r="AJ176" s="21">
+        <v>4</v>
+      </c>
+      <c r="AO176" s="21">
+        <v>1</v>
+      </c>
+      <c r="AP176" s="21">
+        <v>1</v>
+      </c>
+      <c r="AQ176" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:32" s="21" customFormat="1">
+      <c r="A177" s="21">
+        <v>0</v>
+      </c>
+      <c r="B177" s="21">
+        <v>2</v>
+      </c>
+      <c r="C177" s="21">
+        <v>4</v>
+      </c>
+      <c r="D177" s="21">
+        <v>1</v>
+      </c>
+      <c r="E177" s="21">
+        <v>0</v>
+      </c>
+      <c r="F177" s="21">
+        <v>1</v>
+      </c>
+      <c r="I177" s="21">
+        <v>0</v>
+      </c>
+      <c r="J177" s="21">
+        <v>0</v>
+      </c>
+      <c r="K177" s="21">
+        <v>1</v>
+      </c>
+      <c r="L177" s="21">
+        <v>1</v>
+      </c>
+      <c r="M177" s="21">
+        <v>2</v>
+      </c>
+      <c r="N177" s="21">
+        <v>4</v>
+      </c>
       <c r="P177" s="22"/>
-      <c r="Q177" s="23"/>
-      <c r="R177" s="23"/>
-      <c r="S177" s="23"/>
-      <c r="T177" s="23"/>
-      <c r="U177" s="23"/>
-      <c r="V177" s="23"/>
+      <c r="Q177" s="23">
+        <v>0</v>
+      </c>
+      <c r="R177" s="23">
+        <v>0</v>
+      </c>
+      <c r="S177" s="23">
+        <v>0</v>
+      </c>
+      <c r="T177" s="23">
+        <v>0</v>
+      </c>
+      <c r="U177" s="23">
+        <v>0</v>
+      </c>
+      <c r="V177" s="23">
+        <v>0</v>
+      </c>
       <c r="W177" s="23"/>
       <c r="X177" s="23"/>
       <c r="Y177" s="23"/>
@@ -22631,7 +22810,7 @@
       <c r="AD177" s="23"/>
       <c r="AF177" s="39"/>
     </row>
-    <row r="178" spans="16:32" s="21" customFormat="1">
+    <row r="178" spans="1:32" s="21" customFormat="1">
       <c r="P178" s="22"/>
       <c r="Q178" s="23"/>
       <c r="R178" s="23"/>
@@ -22649,25 +22828,25 @@
       <c r="AD178" s="23"/>
       <c r="AF178" s="39"/>
     </row>
-    <row r="179" spans="16:32" s="21" customFormat="1">
+    <row r="179" spans="1:32" s="21" customFormat="1">
       <c r="P179" s="22"/>
-      <c r="Q179" s="23"/>
-      <c r="R179" s="23"/>
-      <c r="S179" s="23"/>
-      <c r="T179" s="23"/>
-      <c r="U179" s="23"/>
-      <c r="V179" s="23"/>
-      <c r="W179" s="23"/>
-      <c r="X179" s="23"/>
-      <c r="Y179" s="23"/>
-      <c r="Z179" s="23"/>
-      <c r="AA179" s="23"/>
-      <c r="AB179" s="23"/>
-      <c r="AC179" s="23"/>
-      <c r="AD179" s="23"/>
+      <c r="Q179" s="20"/>
+      <c r="R179" s="20"/>
+      <c r="S179" s="20"/>
+      <c r="T179" s="20"/>
+      <c r="U179" s="20"/>
+      <c r="V179" s="20"/>
+      <c r="W179" s="15"/>
+      <c r="X179" s="15"/>
+      <c r="Y179" s="15"/>
+      <c r="Z179" s="15"/>
+      <c r="AA179" s="15"/>
+      <c r="AB179" s="15"/>
+      <c r="AC179" s="15"/>
+      <c r="AD179" s="20"/>
       <c r="AF179" s="39"/>
     </row>
-    <row r="180" spans="16:32" s="21" customFormat="1">
+    <row r="180" spans="1:32" s="21" customFormat="1">
       <c r="P180" s="22"/>
       <c r="Q180" s="23"/>
       <c r="R180" s="23"/>
@@ -22676,34 +22855,34 @@
       <c r="U180" s="23"/>
       <c r="V180" s="23"/>
       <c r="W180" s="23"/>
-      <c r="X180" s="23"/>
-      <c r="Y180" s="23"/>
-      <c r="Z180" s="23"/>
-      <c r="AA180" s="23"/>
-      <c r="AB180" s="23"/>
-      <c r="AC180" s="23"/>
+      <c r="X180" s="39"/>
+      <c r="Y180" s="39"/>
+      <c r="Z180" s="39"/>
+      <c r="AA180" s="39"/>
+      <c r="AB180" s="39"/>
+      <c r="AC180" s="39"/>
       <c r="AD180" s="23"/>
       <c r="AF180" s="39"/>
     </row>
-    <row r="181" spans="16:32" s="21" customFormat="1">
+    <row r="181" spans="1:32" s="21" customFormat="1">
       <c r="P181" s="22"/>
-      <c r="Q181" s="20"/>
-      <c r="R181" s="20"/>
-      <c r="S181" s="20"/>
-      <c r="T181" s="20"/>
-      <c r="U181" s="20"/>
-      <c r="V181" s="20"/>
-      <c r="W181" s="15"/>
-      <c r="X181" s="15"/>
-      <c r="Y181" s="15"/>
-      <c r="Z181" s="15"/>
-      <c r="AA181" s="15"/>
-      <c r="AB181" s="15"/>
-      <c r="AC181" s="15"/>
-      <c r="AD181" s="20"/>
+      <c r="Q181" s="23"/>
+      <c r="R181" s="23"/>
+      <c r="S181" s="23"/>
+      <c r="T181" s="23"/>
+      <c r="U181" s="23"/>
+      <c r="V181" s="23"/>
+      <c r="W181" s="23"/>
+      <c r="X181" s="39"/>
+      <c r="Y181" s="39"/>
+      <c r="Z181" s="23"/>
+      <c r="AA181" s="23"/>
+      <c r="AB181" s="23"/>
+      <c r="AC181" s="23"/>
+      <c r="AD181" s="23"/>
       <c r="AF181" s="39"/>
     </row>
-    <row r="182" spans="16:32" s="21" customFormat="1">
+    <row r="182" spans="1:32" s="21" customFormat="1">
       <c r="P182" s="22"/>
       <c r="Q182" s="23"/>
       <c r="R182" s="23"/>
@@ -22711,7 +22890,7 @@
       <c r="T182" s="23"/>
       <c r="U182" s="23"/>
       <c r="V182" s="23"/>
-      <c r="W182" s="23"/>
+      <c r="W182" s="39"/>
       <c r="X182" s="39"/>
       <c r="Y182" s="39"/>
       <c r="Z182" s="39"/>
@@ -22721,25 +22900,24 @@
       <c r="AD182" s="23"/>
       <c r="AF182" s="39"/>
     </row>
-    <row r="183" spans="16:32" s="21" customFormat="1">
-      <c r="P183" s="22"/>
+    <row r="183" spans="1:32" s="21" customFormat="1">
       <c r="Q183" s="23"/>
       <c r="R183" s="23"/>
       <c r="S183" s="23"/>
       <c r="T183" s="23"/>
       <c r="U183" s="23"/>
       <c r="V183" s="23"/>
-      <c r="W183" s="23"/>
+      <c r="W183" s="39"/>
       <c r="X183" s="39"/>
       <c r="Y183" s="39"/>
-      <c r="Z183" s="23"/>
-      <c r="AA183" s="23"/>
-      <c r="AB183" s="23"/>
-      <c r="AC183" s="23"/>
+      <c r="Z183" s="39"/>
+      <c r="AA183" s="39"/>
+      <c r="AB183" s="39"/>
+      <c r="AC183" s="39"/>
       <c r="AD183" s="23"/>
       <c r="AF183" s="39"/>
     </row>
-    <row r="184" spans="16:32" s="21" customFormat="1">
+    <row r="184" spans="1:32" s="21" customFormat="1">
       <c r="P184" s="22"/>
       <c r="Q184" s="23"/>
       <c r="R184" s="23"/>
@@ -22757,7 +22935,7 @@
       <c r="AD184" s="23"/>
       <c r="AF184" s="39"/>
     </row>
-    <row r="185" spans="16:32" s="21" customFormat="1">
+    <row r="185" spans="1:32" s="21" customFormat="1">
       <c r="Q185" s="23"/>
       <c r="R185" s="23"/>
       <c r="S185" s="23"/>
@@ -22774,60 +22952,60 @@
       <c r="AD185" s="23"/>
       <c r="AF185" s="39"/>
     </row>
-    <row r="186" spans="16:32" s="21" customFormat="1">
+    <row r="186" spans="1:32" s="21" customFormat="1">
       <c r="P186" s="22"/>
-      <c r="Q186" s="23"/>
-      <c r="R186" s="23"/>
-      <c r="S186" s="23"/>
-      <c r="T186" s="23"/>
-      <c r="U186" s="23"/>
-      <c r="V186" s="23"/>
-      <c r="W186" s="39"/>
-      <c r="X186" s="39"/>
-      <c r="Y186" s="39"/>
-      <c r="Z186" s="39"/>
-      <c r="AA186" s="39"/>
-      <c r="AB186" s="39"/>
-      <c r="AC186" s="39"/>
-      <c r="AD186" s="23"/>
+      <c r="Q186" s="20"/>
+      <c r="R186" s="20"/>
+      <c r="S186" s="20"/>
+      <c r="T186" s="20"/>
+      <c r="U186" s="20"/>
+      <c r="V186" s="20"/>
+      <c r="W186" s="20"/>
+      <c r="X186" s="20"/>
+      <c r="Y186" s="20"/>
+      <c r="Z186" s="20"/>
+      <c r="AA186" s="20"/>
+      <c r="AB186" s="20"/>
+      <c r="AC186" s="20"/>
+      <c r="AD186" s="20"/>
       <c r="AF186" s="39"/>
     </row>
-    <row r="187" spans="16:32" s="21" customFormat="1">
+    <row r="187" spans="1:32" s="21" customFormat="1">
       <c r="Q187" s="23"/>
       <c r="R187" s="23"/>
       <c r="S187" s="23"/>
       <c r="T187" s="23"/>
       <c r="U187" s="23"/>
       <c r="V187" s="23"/>
-      <c r="W187" s="39"/>
+      <c r="W187" s="23"/>
       <c r="X187" s="39"/>
       <c r="Y187" s="39"/>
-      <c r="Z187" s="39"/>
-      <c r="AA187" s="39"/>
-      <c r="AB187" s="39"/>
-      <c r="AC187" s="39"/>
+      <c r="Z187" s="23"/>
+      <c r="AA187" s="23"/>
+      <c r="AB187" s="23"/>
+      <c r="AC187" s="23"/>
       <c r="AD187" s="23"/>
       <c r="AF187" s="39"/>
     </row>
-    <row r="188" spans="16:32" s="21" customFormat="1">
+    <row r="188" spans="1:32" s="21" customFormat="1">
       <c r="P188" s="22"/>
-      <c r="Q188" s="20"/>
-      <c r="R188" s="20"/>
-      <c r="S188" s="20"/>
-      <c r="T188" s="20"/>
-      <c r="U188" s="20"/>
-      <c r="V188" s="20"/>
-      <c r="W188" s="20"/>
-      <c r="X188" s="20"/>
-      <c r="Y188" s="20"/>
-      <c r="Z188" s="20"/>
-      <c r="AA188" s="20"/>
-      <c r="AB188" s="20"/>
-      <c r="AC188" s="20"/>
-      <c r="AD188" s="20"/>
+      <c r="Q188" s="23"/>
+      <c r="R188" s="23"/>
+      <c r="S188" s="23"/>
+      <c r="T188" s="23"/>
+      <c r="U188" s="23"/>
+      <c r="V188" s="23"/>
+      <c r="W188" s="39"/>
+      <c r="X188" s="39"/>
+      <c r="Y188" s="39"/>
+      <c r="Z188" s="39"/>
+      <c r="AA188" s="39"/>
+      <c r="AB188" s="39"/>
+      <c r="AC188" s="39"/>
+      <c r="AD188" s="23"/>
       <c r="AF188" s="39"/>
     </row>
-    <row r="189" spans="16:32" s="21" customFormat="1">
+    <row r="189" spans="1:32" s="21" customFormat="1">
       <c r="Q189" s="23"/>
       <c r="R189" s="23"/>
       <c r="S189" s="23"/>
@@ -22844,7 +23022,7 @@
       <c r="AD189" s="23"/>
       <c r="AF189" s="39"/>
     </row>
-    <row r="190" spans="16:32" s="21" customFormat="1">
+    <row r="190" spans="1:32" s="21" customFormat="1">
       <c r="P190" s="22"/>
       <c r="Q190" s="23"/>
       <c r="R190" s="23"/>
@@ -22852,126 +23030,91 @@
       <c r="T190" s="23"/>
       <c r="U190" s="23"/>
       <c r="V190" s="23"/>
-      <c r="W190" s="39"/>
-      <c r="X190" s="39"/>
-      <c r="Y190" s="39"/>
-      <c r="Z190" s="39"/>
-      <c r="AA190" s="39"/>
-      <c r="AB190" s="39"/>
-      <c r="AC190" s="39"/>
+      <c r="W190" s="23"/>
+      <c r="X190" s="23"/>
+      <c r="Y190" s="23"/>
+      <c r="Z190" s="23"/>
+      <c r="AA190" s="23"/>
+      <c r="AB190" s="23"/>
+      <c r="AC190" s="23"/>
       <c r="AD190" s="23"/>
       <c r="AF190" s="39"/>
     </row>
-    <row r="191" spans="16:32" s="21" customFormat="1">
-      <c r="Q191" s="23"/>
-      <c r="R191" s="23"/>
-      <c r="S191" s="23"/>
-      <c r="T191" s="23"/>
-      <c r="U191" s="23"/>
-      <c r="V191" s="23"/>
-      <c r="W191" s="23"/>
-      <c r="X191" s="39"/>
-      <c r="Y191" s="39"/>
-      <c r="Z191" s="23"/>
-      <c r="AA191" s="23"/>
-      <c r="AB191" s="23"/>
-      <c r="AC191" s="23"/>
-      <c r="AD191" s="23"/>
+    <row r="191" spans="1:32" s="21" customFormat="1">
+      <c r="P191" s="22"/>
+      <c r="Q191" s="20"/>
+      <c r="R191" s="20"/>
+      <c r="S191" s="20"/>
+      <c r="T191" s="20"/>
+      <c r="U191" s="20"/>
+      <c r="V191" s="20"/>
+      <c r="W191" s="20"/>
+      <c r="X191" s="20"/>
+      <c r="Y191" s="20"/>
+      <c r="Z191" s="20"/>
+      <c r="AA191" s="20"/>
+      <c r="AB191" s="20"/>
+      <c r="AC191" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD191" s="20"/>
       <c r="AF191" s="39"/>
     </row>
-    <row r="192" spans="16:32" s="21" customFormat="1">
+    <row r="192" spans="1:32" s="21" customFormat="1">
       <c r="P192" s="22"/>
-      <c r="Q192" s="23"/>
-      <c r="R192" s="23"/>
-      <c r="S192" s="23"/>
-      <c r="T192" s="23"/>
-      <c r="U192" s="23"/>
-      <c r="V192" s="23"/>
-      <c r="W192" s="23"/>
-      <c r="X192" s="23"/>
-      <c r="Y192" s="23"/>
-      <c r="Z192" s="23"/>
-      <c r="AA192" s="23"/>
-      <c r="AB192" s="23"/>
-      <c r="AC192" s="23"/>
-      <c r="AD192" s="23"/>
+      <c r="Q192" s="20"/>
+      <c r="R192" s="20"/>
+      <c r="S192" s="20"/>
+      <c r="T192" s="20"/>
+      <c r="U192" s="20"/>
+      <c r="V192" s="20"/>
+      <c r="W192" s="20"/>
+      <c r="X192" s="20"/>
+      <c r="Y192" s="20"/>
+      <c r="Z192" s="20"/>
+      <c r="AA192" s="20"/>
+      <c r="AB192" s="20"/>
+      <c r="AC192" s="20"/>
+      <c r="AD192" s="20"/>
       <c r="AF192" s="39"/>
     </row>
-    <row r="193" spans="9:32" s="21" customFormat="1">
-      <c r="I193" s="21">
-        <v>0</v>
-      </c>
-      <c r="J193" s="21">
-        <v>1</v>
-      </c>
-      <c r="K193" s="21">
-        <v>2</v>
-      </c>
-      <c r="L193" s="21">
-        <v>5</v>
-      </c>
-      <c r="M193" s="21">
-        <v>5</v>
-      </c>
-      <c r="N193" s="21">
-        <v>7</v>
-      </c>
+    <row r="193" spans="16:32" s="21" customFormat="1">
       <c r="P193" s="22"/>
-      <c r="Q193" s="20"/>
-      <c r="R193" s="20"/>
-      <c r="S193" s="20"/>
-      <c r="T193" s="20"/>
-      <c r="U193" s="20"/>
-      <c r="V193" s="20"/>
-      <c r="W193" s="20"/>
-      <c r="X193" s="20"/>
-      <c r="Y193" s="20"/>
-      <c r="Z193" s="20"/>
-      <c r="AA193" s="20"/>
-      <c r="AB193" s="20"/>
-      <c r="AC193" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD193" s="20"/>
+      <c r="Q193" s="23"/>
+      <c r="R193" s="23"/>
+      <c r="S193" s="23"/>
+      <c r="T193" s="23"/>
+      <c r="U193" s="23"/>
+      <c r="V193" s="23"/>
+      <c r="W193" s="23"/>
+      <c r="X193" s="23"/>
+      <c r="Y193" s="23"/>
+      <c r="Z193" s="23"/>
+      <c r="AA193" s="23"/>
+      <c r="AB193" s="23"/>
+      <c r="AC193" s="23"/>
+      <c r="AD193" s="23"/>
       <c r="AF193" s="39"/>
     </row>
-    <row r="194" spans="9:32" s="21" customFormat="1">
-      <c r="I194" s="21">
-        <v>0</v>
-      </c>
-      <c r="J194" s="21">
-        <v>1</v>
-      </c>
-      <c r="K194" s="21">
-        <v>3</v>
-      </c>
-      <c r="L194" s="21">
-        <v>3</v>
-      </c>
-      <c r="M194" s="21">
-        <v>6</v>
-      </c>
-      <c r="N194" s="21">
-        <v>6</v>
-      </c>
+    <row r="194" spans="16:32" s="21" customFormat="1">
       <c r="P194" s="22"/>
-      <c r="Q194" s="20"/>
-      <c r="R194" s="20"/>
-      <c r="S194" s="20"/>
-      <c r="T194" s="20"/>
-      <c r="U194" s="20"/>
-      <c r="V194" s="20"/>
-      <c r="W194" s="20"/>
-      <c r="X194" s="20"/>
-      <c r="Y194" s="20"/>
-      <c r="Z194" s="20"/>
-      <c r="AA194" s="20"/>
-      <c r="AB194" s="20"/>
-      <c r="AC194" s="20"/>
-      <c r="AD194" s="20"/>
+      <c r="Q194" s="23"/>
+      <c r="R194" s="23"/>
+      <c r="S194" s="23"/>
+      <c r="T194" s="23"/>
+      <c r="U194" s="23"/>
+      <c r="V194" s="23"/>
+      <c r="W194" s="23"/>
+      <c r="X194" s="23"/>
+      <c r="Y194" s="23"/>
+      <c r="Z194" s="23"/>
+      <c r="AA194" s="23"/>
+      <c r="AB194" s="23"/>
+      <c r="AC194" s="23"/>
+      <c r="AD194" s="23"/>
       <c r="AF194" s="39"/>
     </row>
-    <row r="195" spans="9:32" s="21" customFormat="1">
+    <row r="195" spans="16:32" s="21" customFormat="1">
       <c r="P195" s="22"/>
       <c r="Q195" s="23"/>
       <c r="R195" s="23"/>
@@ -22989,7 +23132,7 @@
       <c r="AD195" s="23"/>
       <c r="AF195" s="39"/>
     </row>
-    <row r="196" spans="9:32" s="21" customFormat="1">
+    <row r="196" spans="16:32" s="21" customFormat="1">
       <c r="P196" s="22"/>
       <c r="Q196" s="23"/>
       <c r="R196" s="23"/>
@@ -23007,7 +23150,7 @@
       <c r="AD196" s="23"/>
       <c r="AF196" s="39"/>
     </row>
-    <row r="197" spans="9:32" s="21" customFormat="1">
+    <row r="197" spans="16:32" s="21" customFormat="1">
       <c r="P197" s="22"/>
       <c r="Q197" s="23"/>
       <c r="R197" s="23"/>
@@ -23025,7 +23168,7 @@
       <c r="AD197" s="23"/>
       <c r="AF197" s="39"/>
     </row>
-    <row r="198" spans="9:32" s="21" customFormat="1">
+    <row r="198" spans="16:32" s="21" customFormat="1">
       <c r="P198" s="22"/>
       <c r="Q198" s="23"/>
       <c r="R198" s="23"/>
@@ -23043,7 +23186,7 @@
       <c r="AD198" s="23"/>
       <c r="AF198" s="39"/>
     </row>
-    <row r="199" spans="9:32" s="21" customFormat="1">
+    <row r="199" spans="16:32" s="21" customFormat="1">
       <c r="P199" s="22"/>
       <c r="Q199" s="23"/>
       <c r="R199" s="23"/>
@@ -23061,7 +23204,7 @@
       <c r="AD199" s="23"/>
       <c r="AF199" s="39"/>
     </row>
-    <row r="200" spans="9:32" s="21" customFormat="1">
+    <row r="200" spans="16:32" s="21" customFormat="1">
       <c r="Q200" s="23"/>
       <c r="R200" s="23"/>
       <c r="S200" s="23"/>
@@ -23078,7 +23221,7 @@
       <c r="AD200" s="23"/>
       <c r="AF200" s="39"/>
     </row>
-    <row r="201" spans="9:32" s="21" customFormat="1">
+    <row r="201" spans="16:32" s="21" customFormat="1">
       <c r="Q201" s="23"/>
       <c r="R201" s="23"/>
       <c r="S201" s="23"/>
@@ -23095,7 +23238,7 @@
       <c r="AD201" s="23"/>
       <c r="AF201" s="39"/>
     </row>
-    <row r="202" spans="9:32">
+    <row r="202" spans="16:32">
       <c r="Q202" s="39"/>
       <c r="R202" s="39"/>
       <c r="S202" s="39"/>
@@ -23112,7 +23255,7 @@
       <c r="AD202" s="23"/>
       <c r="AF202" s="39"/>
     </row>
-    <row r="203" spans="9:32" s="21" customFormat="1">
+    <row r="203" spans="16:32" s="21" customFormat="1">
       <c r="P203" s="22"/>
       <c r="Q203" s="23"/>
       <c r="R203" s="23"/>
@@ -23130,7 +23273,7 @@
       <c r="AD203" s="23"/>
       <c r="AF203" s="39"/>
     </row>
-    <row r="204" spans="9:32" s="21" customFormat="1">
+    <row r="204" spans="16:32" s="21" customFormat="1">
       <c r="Q204" s="23"/>
       <c r="R204" s="23"/>
       <c r="S204" s="23"/>
@@ -23147,7 +23290,7 @@
       <c r="AD204" s="23"/>
       <c r="AF204" s="39"/>
     </row>
-    <row r="205" spans="9:32" s="21" customFormat="1">
+    <row r="205" spans="16:32" s="21" customFormat="1">
       <c r="Q205" s="23"/>
       <c r="R205" s="23"/>
       <c r="S205" s="23"/>
@@ -23164,7 +23307,7 @@
       <c r="AD205" s="23"/>
       <c r="AF205" s="39"/>
     </row>
-    <row r="206" spans="9:32" s="21" customFormat="1">
+    <row r="206" spans="16:32" s="21" customFormat="1">
       <c r="Q206" s="23"/>
       <c r="R206" s="23"/>
       <c r="S206" s="23"/>
@@ -23181,7 +23324,7 @@
       <c r="AD206" s="23"/>
       <c r="AF206" s="39"/>
     </row>
-    <row r="207" spans="9:32" s="21" customFormat="1">
+    <row r="207" spans="16:32" s="21" customFormat="1">
       <c r="Q207" s="23"/>
       <c r="R207" s="23"/>
       <c r="S207" s="23"/>
@@ -23198,7 +23341,7 @@
       <c r="AD207" s="23"/>
       <c r="AF207" s="39"/>
     </row>
-    <row r="208" spans="9:32" s="21" customFormat="1">
+    <row r="208" spans="16:32" s="21" customFormat="1">
       <c r="P208" s="22"/>
       <c r="Q208" s="23"/>
       <c r="R208" s="23"/>
@@ -35051,8 +35194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO243"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H183" sqref="H183"/>
+    <sheetView topLeftCell="A155" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D184" sqref="D184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.625" defaultRowHeight="13.5"/>
@@ -38737,19 +38880,43 @@
       </c>
     </row>
     <row r="176" spans="1:22">
-      <c r="A176" s="10"/>
+      <c r="A176" s="9">
+        <v>1</v>
+      </c>
       <c r="B176" s="10"/>
-      <c r="C176" s="10"/>
+      <c r="C176" s="9">
+        <v>1</v>
+      </c>
       <c r="D176" s="10"/>
-      <c r="E176" s="10"/>
+      <c r="E176" s="11">
+        <v>4</v>
+      </c>
       <c r="F176" s="10"/>
+      <c r="G176" s="18"/>
+      <c r="H176" s="18"/>
+      <c r="I176" s="18"/>
+      <c r="J176" s="18"/>
+      <c r="K176" s="18"/>
+      <c r="L176" s="18"/>
+      <c r="M176" s="18"/>
+      <c r="N176" s="18"/>
+      <c r="O176" s="18"/>
+      <c r="P176" s="10"/>
     </row>
     <row r="177" spans="1:6">
-      <c r="A177" s="10"/>
-      <c r="B177" s="10"/>
-      <c r="C177" s="10"/>
+      <c r="A177" s="11">
+        <v>2</v>
+      </c>
+      <c r="B177" s="11">
+        <v>2</v>
+      </c>
+      <c r="C177" s="9">
+        <v>1</v>
+      </c>
       <c r="D177" s="10"/>
-      <c r="E177" s="10"/>
+      <c r="E177" s="9">
+        <v>1</v>
+      </c>
       <c r="F177" s="10"/>
     </row>
     <row r="178" spans="1:6">
@@ -38933,6 +39100,7 @@
       <c r="B200" s="10"/>
       <c r="C200" s="10"/>
       <c r="D200" s="10"/>
+      <c r="E200" s="10"/>
       <c r="F200" s="10"/>
     </row>
     <row r="201" spans="1:6">
@@ -39084,11 +39252,13 @@
     </row>
     <row r="223" spans="1:6">
       <c r="A223" s="10"/>
+      <c r="B223" s="10"/>
       <c r="C223" s="10"/>
       <c r="D223" s="10"/>
     </row>
     <row r="224" spans="1:6">
       <c r="A224" s="10"/>
+      <c r="B224" s="10"/>
       <c r="C224" s="10"/>
       <c r="D224" s="10"/>
     </row>
@@ -39140,8 +39310,10 @@
     <row r="234" spans="1:4">
       <c r="A234" s="10"/>
       <c r="C234" s="10"/>
+      <c r="D234" s="10"/>
     </row>
     <row r="235" spans="1:4">
+      <c r="A235" s="10"/>
       <c r="C235" s="10"/>
     </row>
     <row r="236" spans="1:4">
@@ -39179,8 +39351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U197"/>
   <sheetViews>
-    <sheetView topLeftCell="A150" workbookViewId="0">
-      <selection activeCell="M181" sqref="M181"/>
+    <sheetView topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="L186" sqref="L186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -43738,7 +43910,101 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="14:19" customFormat="1">
+    <row r="176" spans="1:19">
+      <c r="A176" s="1">
+        <v>1</v>
+      </c>
+      <c r="B176" s="1">
+        <v>2</v>
+      </c>
+      <c r="C176" s="1">
+        <v>3</v>
+      </c>
+      <c r="F176" s="1">
+        <v>1</v>
+      </c>
+      <c r="G176" s="1">
+        <v>2</v>
+      </c>
+      <c r="H176" s="1">
+        <v>1</v>
+      </c>
+      <c r="I176" s="1">
+        <v>0</v>
+      </c>
+      <c r="J176" s="1">
+        <v>0</v>
+      </c>
+      <c r="K176" s="1">
+        <v>2</v>
+      </c>
+      <c r="N176" s="1">
+        <v>0</v>
+      </c>
+      <c r="O176" s="1">
+        <v>0</v>
+      </c>
+      <c r="P176" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q176" s="1">
+        <v>2</v>
+      </c>
+      <c r="R176" s="1">
+        <v>13</v>
+      </c>
+      <c r="S176" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19">
+      <c r="A177" s="1">
+        <v>2</v>
+      </c>
+      <c r="B177" s="1">
+        <v>2</v>
+      </c>
+      <c r="C177" s="1">
+        <v>2</v>
+      </c>
+      <c r="F177" s="1">
+        <v>2</v>
+      </c>
+      <c r="G177" s="1">
+        <v>0</v>
+      </c>
+      <c r="H177" s="1">
+        <v>1</v>
+      </c>
+      <c r="I177" s="1">
+        <v>1</v>
+      </c>
+      <c r="J177" s="1">
+        <v>2</v>
+      </c>
+      <c r="K177" s="1">
+        <v>0</v>
+      </c>
+      <c r="N177" s="1">
+        <v>0</v>
+      </c>
+      <c r="O177" s="1">
+        <v>1</v>
+      </c>
+      <c r="P177" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q177" s="1">
+        <v>4</v>
+      </c>
+      <c r="R177" s="1">
+        <v>5</v>
+      </c>
+      <c r="S177" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182" spans="1:19" customFormat="1">
       <c r="N182" s="18"/>
       <c r="O182" s="18"/>
       <c r="P182" s="18"/>
@@ -43771,10 +44037,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A100:AN175"/>
+  <dimension ref="A100:AN177"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="I180" sqref="I180"/>
+    <sheetView topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="K183" sqref="K183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -47207,6 +47473,82 @@
         <v>2</v>
       </c>
     </row>
+    <row r="176" spans="1:19">
+      <c r="A176" s="9">
+        <v>1</v>
+      </c>
+      <c r="D176" s="9">
+        <v>1</v>
+      </c>
+      <c r="F176" s="11">
+        <v>2</v>
+      </c>
+      <c r="G176" s="9">
+        <v>1</v>
+      </c>
+      <c r="J176" s="9">
+        <v>1</v>
+      </c>
+      <c r="L176" s="16">
+        <v>0</v>
+      </c>
+      <c r="M176" s="16">
+        <v>1</v>
+      </c>
+      <c r="N176" s="16">
+        <v>4</v>
+      </c>
+      <c r="O176" s="16">
+        <v>6</v>
+      </c>
+      <c r="P176" s="16">
+        <v>6</v>
+      </c>
+      <c r="Q176" s="16">
+        <v>7</v>
+      </c>
+      <c r="S176" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="177" spans="1:19">
+      <c r="A177" s="9">
+        <v>1</v>
+      </c>
+      <c r="B177" s="9">
+        <v>1</v>
+      </c>
+      <c r="C177" s="9">
+        <v>1</v>
+      </c>
+      <c r="G177" s="11">
+        <v>2</v>
+      </c>
+      <c r="I177" s="9">
+        <v>1</v>
+      </c>
+      <c r="L177" s="16">
+        <v>1</v>
+      </c>
+      <c r="M177" s="16">
+        <v>2</v>
+      </c>
+      <c r="N177" s="16">
+        <v>3</v>
+      </c>
+      <c r="O177" s="16">
+        <v>7</v>
+      </c>
+      <c r="P177" s="16">
+        <v>7</v>
+      </c>
+      <c r="Q177" s="16">
+        <v>9</v>
+      </c>
+      <c r="S177" s="16">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -47219,7 +47561,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -47443,7 +47785,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="18">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="18">
         <v>15</v>
@@ -47578,10 +47920,10 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="18">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="18">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" s="19">
         <v>6</v>
@@ -47684,7 +48026,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K10" s="18">
         <v>1</v>
@@ -47693,7 +48035,7 @@
         <v>21</v>
       </c>
       <c r="M10" s="18">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N10" s="18">
         <v>1</v>
@@ -47710,7 +48052,7 @@
         <v>35</v>
       </c>
       <c r="E11" s="18">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F11" s="19">
         <v>11</v>
@@ -47719,11 +48061,14 @@
         <v>48</v>
       </c>
       <c r="H11" s="18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I11" s="18">
         <v>11</v>
       </c>
+      <c r="J11" s="18">
+        <v>0</v>
+      </c>
       <c r="K11" s="18">
         <v>20</v>
       </c>
@@ -47734,18 +48079,21 @@
         <v>12</v>
       </c>
       <c r="O11" s="18">
+        <v>3</v>
+      </c>
+      <c r="P11" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="C12" s="19">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F12" s="19">
         <v>9</v>
       </c>
       <c r="G12" s="18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12" s="18">
         <v>19</v>
@@ -47771,7 +48119,7 @@
         <v>14</v>
       </c>
       <c r="L13" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="18">
         <v>0</v>
@@ -47782,18 +48130,18 @@
         <v>29</v>
       </c>
       <c r="I14" s="18">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K14" s="18">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N14" s="18">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="F15" s="19">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -47807,7 +48155,7 @@
   <dimension ref="A2:AG24"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -48087,4 +48435,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>